<commit_message>
docs(*):Supplement additional test datas that include 10 samples in each level
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonCode\Sodoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7A174A-3434-4107-AB2E-527F62F1302B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19E75A-D048-4C44-BD3B-D95ACAF4E0AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,16 +336,16 @@
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>128.33333333333334</c:v>
+                  <c:v>131.30000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>188.66666666666666</c:v>
+                  <c:v>185.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>243</c:v>
+                  <c:v>238.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>262</c:v>
+                  <c:v>270.60000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,16 +357,16 @@
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.7966666666666666</c:v>
+                  <c:v>5.5620000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8833333333333337</c:v>
+                  <c:v>16.922999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>132.07</c:v>
+                  <c:v>179.83599999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>537.97333333333336</c:v>
+                  <c:v>609.16199999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -375,6 +375,386 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-589A-464B-8628-C2A455A327A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="544785408"/>
+        <c:axId val="544777864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="544785408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00_);[Red]\(0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544777864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="544777864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00_);[Red]\(0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544785408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Step</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Basic!$D$2,Basic!$I$2,Basic!$N$2,Basic!$S$2)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>131.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>185.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>238.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>270.60000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Basic!$B$2,Basic!$G$2,Basic!$L$2,Basic!$Q$2)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>383.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1336.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13954.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47744.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4812-4BD1-B0D3-B2D9367E45BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -620,6 +1000,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
@@ -1169,20 +1589,569 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>146304</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>54864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1202,6 +2171,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>21336</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC022FCD-D58E-4F3E-B098-93973C7D21E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1475,14 +2482,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="5" max="5" width="2.6640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="2.88671875" style="3" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
@@ -1524,67 +2531,67 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f t="shared" ref="A2:C2" si="0">AVERAGE(A4:A30)</f>
-        <v>1.7966666666666666</v>
+        <v>5.5620000000000003</v>
       </c>
       <c r="B2" s="7">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>383.7</v>
       </c>
       <c r="C2" s="7">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>40.1</v>
       </c>
       <c r="D2" s="7">
         <f>AVERAGE(D4:D30)</f>
-        <v>128.33333333333334</v>
+        <v>131.30000000000001</v>
       </c>
       <c r="F2" s="7">
         <f>AVERAGE(F4:F51)</f>
-        <v>4.8833333333333337</v>
+        <v>16.922999999999998</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" ref="G2:I2" si="1">AVERAGE(G4:G51)</f>
-        <v>389.33333333333331</v>
+        <v>1336.8</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" si="1"/>
-        <v>47.333333333333336</v>
+        <v>47.8</v>
       </c>
       <c r="I2" s="7">
         <f t="shared" si="1"/>
-        <v>188.66666666666666</v>
+        <v>185.9</v>
       </c>
       <c r="K2" s="7">
         <f>AVERAGE(K4:K80)</f>
-        <v>132.07</v>
+        <v>179.83599999999996</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" ref="L2:N2" si="2">AVERAGE(L4:L80)</f>
-        <v>9755</v>
+        <v>13954.5</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" si="2"/>
-        <v>53.5</v>
+        <v>53.6</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" si="2"/>
-        <v>243</v>
+        <v>238.9</v>
       </c>
       <c r="P2" s="7">
         <f>AVERAGE(P4:P800)</f>
-        <v>537.97333333333336</v>
+        <v>609.16199999999992</v>
       </c>
       <c r="Q2" s="7">
         <f t="shared" ref="Q2:S2" si="3">AVERAGE(Q4:Q800)</f>
-        <v>41060.333333333336</v>
+        <v>47744.6</v>
       </c>
       <c r="R2" s="7">
         <f t="shared" si="3"/>
-        <v>55.666666666666664</v>
+        <v>56.4</v>
       </c>
       <c r="S2" s="7">
         <f t="shared" si="3"/>
-        <v>262</v>
+        <v>270.60000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1643,7 +2650,7 @@
     </row>
     <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>1.41</v>
+        <v>1.34</v>
       </c>
       <c r="B4" s="5">
         <v>95</v>
@@ -1652,7 +2659,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="5">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="5">
@@ -1697,7 +2704,7 @@
     </row>
     <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>1.91</v>
+        <v>2.25</v>
       </c>
       <c r="B5" s="5">
         <v>149</v>
@@ -1706,7 +2713,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="5">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5">
@@ -1751,7 +2758,7 @@
     </row>
     <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>2.0699999999999998</v>
+        <v>2.15</v>
       </c>
       <c r="B6" s="5">
         <v>149</v>
@@ -1760,7 +2767,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="5">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5">
@@ -1804,7 +2811,31 @@
       <c r="T6" s="6"/>
     </row>
     <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2.72</v>
+      </c>
+      <c r="B7" s="5">
+        <v>203</v>
+      </c>
+      <c r="C7" s="5">
+        <v>41</v>
+      </c>
+      <c r="D7" s="5">
+        <v>123</v>
+      </c>
       <c r="E7" s="6"/>
+      <c r="F7" s="5">
+        <v>30.14</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2191</v>
+      </c>
+      <c r="H7" s="5">
+        <v>48</v>
+      </c>
+      <c r="I7" s="5">
+        <v>186</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="5">
         <v>68.81</v>
@@ -1819,42 +2850,342 @@
         <v>237</v>
       </c>
       <c r="O7" s="6"/>
+      <c r="P7" s="5">
+        <v>998.24</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>79402</v>
+      </c>
+      <c r="R7" s="5">
+        <v>57</v>
+      </c>
+      <c r="S7" s="5">
+        <v>273</v>
+      </c>
       <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>2.02</v>
+      </c>
+      <c r="B8" s="5">
+        <v>141</v>
+      </c>
+      <c r="C8" s="5">
+        <v>41</v>
+      </c>
+      <c r="D8" s="5">
+        <v>142</v>
+      </c>
       <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G8" s="5">
+        <v>382</v>
+      </c>
+      <c r="H8" s="5">
+        <v>48</v>
+      </c>
+      <c r="I8" s="5">
+        <v>189</v>
+      </c>
       <c r="J8" s="6"/>
+      <c r="K8" s="5">
+        <v>95.95</v>
+      </c>
+      <c r="L8" s="5">
+        <v>7599</v>
+      </c>
+      <c r="M8" s="5">
+        <v>54</v>
+      </c>
+      <c r="N8" s="5">
+        <v>249</v>
+      </c>
       <c r="O8" s="6"/>
+      <c r="P8" s="5">
+        <v>88.18</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>6976</v>
+      </c>
+      <c r="R8" s="5">
+        <v>55</v>
+      </c>
+      <c r="S8" s="5">
+        <v>253</v>
+      </c>
       <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>2.16</v>
+      </c>
+      <c r="B9" s="5">
+        <v>150</v>
+      </c>
+      <c r="C9" s="5">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5">
+        <v>131</v>
+      </c>
       <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <v>12.08</v>
+      </c>
+      <c r="G9" s="5">
+        <v>966</v>
+      </c>
+      <c r="H9" s="5">
+        <v>48</v>
+      </c>
+      <c r="I9" s="5">
+        <v>179</v>
+      </c>
       <c r="J9" s="6"/>
+      <c r="K9" s="5">
+        <v>606.29999999999995</v>
+      </c>
+      <c r="L9" s="5">
+        <v>47664</v>
+      </c>
+      <c r="M9" s="5">
+        <v>54</v>
+      </c>
+      <c r="N9" s="5">
+        <v>239</v>
+      </c>
       <c r="O9" s="6"/>
+      <c r="P9" s="5">
+        <v>2206.7199999999998</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>174368</v>
+      </c>
+      <c r="R9" s="5">
+        <v>57</v>
+      </c>
+      <c r="S9" s="5">
+        <v>267</v>
+      </c>
       <c r="T9" s="6"/>
     </row>
     <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>2.92</v>
+      </c>
+      <c r="B10" s="5">
+        <v>215</v>
+      </c>
+      <c r="C10" s="5">
+        <v>41</v>
+      </c>
+      <c r="D10" s="5">
+        <v>132</v>
+      </c>
       <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1477</v>
+      </c>
+      <c r="H10" s="5">
+        <v>48</v>
+      </c>
+      <c r="I10" s="5">
+        <v>187</v>
+      </c>
       <c r="J10" s="6"/>
+      <c r="K10" s="5">
+        <v>47.36</v>
+      </c>
+      <c r="L10" s="5">
+        <v>3758</v>
+      </c>
+      <c r="M10" s="5">
+        <v>54</v>
+      </c>
+      <c r="N10" s="5">
+        <v>237</v>
+      </c>
       <c r="O10" s="6"/>
+      <c r="P10" s="5">
+        <v>124.42</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>9934</v>
+      </c>
+      <c r="R10" s="5">
+        <v>57</v>
+      </c>
+      <c r="S10" s="5">
+        <v>278</v>
+      </c>
       <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>1.95</v>
+      </c>
+      <c r="B11" s="5">
+        <v>89</v>
+      </c>
+      <c r="C11" s="5">
+        <v>41</v>
+      </c>
+      <c r="D11" s="5">
+        <v>140</v>
+      </c>
       <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <v>15.27</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1229</v>
+      </c>
+      <c r="H11" s="5">
+        <v>48</v>
+      </c>
+      <c r="I11" s="5">
+        <v>184</v>
+      </c>
       <c r="J11" s="6"/>
+      <c r="K11" s="5">
+        <v>324.31</v>
+      </c>
+      <c r="L11" s="5">
+        <v>25593</v>
+      </c>
+      <c r="M11" s="5">
+        <v>54</v>
+      </c>
+      <c r="N11" s="5">
+        <v>238</v>
+      </c>
       <c r="O11" s="6"/>
+      <c r="P11" s="5">
+        <v>837.4</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>66034</v>
+      </c>
+      <c r="R11" s="5">
+        <v>57</v>
+      </c>
+      <c r="S11" s="5">
+        <v>284</v>
+      </c>
       <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="B12" s="5">
+        <v>95</v>
+      </c>
+      <c r="C12" s="5">
+        <v>41</v>
+      </c>
+      <c r="D12" s="5">
+        <v>141</v>
+      </c>
       <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <v>69.47</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5649</v>
+      </c>
+      <c r="H12" s="5">
+        <v>48</v>
+      </c>
+      <c r="I12" s="5">
+        <v>196</v>
+      </c>
       <c r="J12" s="6"/>
+      <c r="K12" s="5">
+        <v>29.78</v>
+      </c>
+      <c r="L12" s="5">
+        <v>2400</v>
+      </c>
+      <c r="M12" s="5">
+        <v>52</v>
+      </c>
+      <c r="N12" s="5">
+        <v>207</v>
+      </c>
       <c r="O12" s="6"/>
+      <c r="P12" s="5">
+        <v>115.99</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>9162</v>
+      </c>
+      <c r="R12" s="5">
+        <v>57</v>
+      </c>
+      <c r="S12" s="5">
+        <v>287</v>
+      </c>
       <c r="T12" s="6"/>
     </row>
     <row r="13" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>36.71</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2551</v>
+      </c>
+      <c r="C13" s="5">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5">
+        <v>146</v>
+      </c>
       <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <v>3.82</v>
+      </c>
+      <c r="G13" s="5">
+        <v>306</v>
+      </c>
+      <c r="H13" s="5">
+        <v>48</v>
+      </c>
+      <c r="I13" s="5">
+        <v>172</v>
+      </c>
       <c r="J13" s="6"/>
+      <c r="K13" s="5">
+        <v>166.38</v>
+      </c>
+      <c r="L13" s="5">
+        <v>13511</v>
+      </c>
+      <c r="M13" s="5">
+        <v>54</v>
+      </c>
+      <c r="N13" s="5">
+        <v>247</v>
+      </c>
       <c r="O13" s="6"/>
+      <c r="P13" s="5">
+        <v>106.75</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>8389</v>
+      </c>
+      <c r="R13" s="5">
+        <v>57</v>
+      </c>
+      <c r="S13" s="5">
+        <v>278</v>
+      </c>
       <c r="T13" s="6"/>
     </row>
     <row r="14" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat(*):Established new optimiziational method————ArrayPlaceholder - Established new uncompleted method which could only deal with case with one candidate
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonCode\Sodoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19E75A-D048-4C44-BD3B-D95ACAF4E0AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74687D5-169D-4393-894F-7E18B9B99DD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2482,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6:X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>